<commit_message>
Add the latest versions of all files
</commit_message>
<xml_diff>
--- a/Risk_List.xlsx
+++ b/Risk_List.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miUmE7hPj8vbBl6s7vBW1JmHfpSbg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgf4lMguMmmbn2wiXizshoCLwis2Q=="/>
     </ext>
   </extLst>
 </workbook>
@@ -62,16 +62,16 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi77esmQKfcahQUfc+uLD6CAVYCvA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mj/XWyqaBi5qYHAWkGXeu0KnCMqDw=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
-    <t>Hotel Reservation System Project Risk List v3.0</t>
+    <t>Hotel Reservation System Project Risk List v4.0</t>
   </si>
   <si>
     <t>Risk ID</t>
@@ -142,7 +142,9 @@
     <t>Analyst</t>
   </si>
   <si>
-    <t>Using different elicitation techniques like prototyping focus group</t>
+    <t xml:space="preserve">Using different elicitation techniques like prototyping focus group
+-&gt; Done. This risk is mitigated. HRS requirements are elaborated during qa review meetings before the eyes of pretending users(i.e qa team)
+</t>
   </si>
   <si>
     <t>Incompatibility with GUI and specific configurations on client machines.</t>
@@ -183,7 +185,27 @@
     <t>Developers may not have enough experienced in programming and face difficulties in constructing.</t>
   </si>
   <si>
-    <t>Select a familiar development libraries and infrastructure.</t>
+    <t>Select a familiar development libraries and infrastructure.
+-&gt; Done. This is risk is mitigated. Developers have adequate experience in order to finalize code implementation.</t>
+  </si>
+  <si>
+    <t>Emergency leave</t>
+  </si>
+  <si>
+    <t>Emergency situation can be occured during development phase. As a result of this, project schedule can be delayed.</t>
+  </si>
+  <si>
+    <t>Overtime for each remaining members are conducted.</t>
+  </si>
+  <si>
+    <t>UI problems</t>
+  </si>
+  <si>
+    <t>Application development environments can output different layouts and other UI related bugs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application development environments must be updated.
+-&gt; Done. Eclipse version is updated. </t>
   </si>
 </sst>
 </file>
@@ -262,12 +284,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -298,6 +320,15 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -705,7 +736,7 @@
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="10"/>
@@ -725,8 +756,8 @@
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
     </row>
-    <row r="5" ht="24.75" customHeight="1">
-      <c r="A5" s="6">
+    <row r="5" ht="81.0" customHeight="1">
+      <c r="A5" s="11">
         <v>3.0</v>
       </c>
       <c r="B5" s="7">
@@ -754,7 +785,7 @@
       <c r="I5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="12" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="10"/>
@@ -871,8 +902,8 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" ht="37.5" customHeight="1">
-      <c r="A8" s="6">
+    <row r="8">
+      <c r="A8" s="11">
         <v>6.0</v>
       </c>
       <c r="B8" s="7">
@@ -900,7 +931,7 @@
       <c r="I8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K8" s="10"/>
@@ -920,22 +951,38 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="6">
+    <row r="9">
+      <c r="A9" s="11">
         <v>7.0</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="8"/>
+      <c r="B9" s="13">
+        <v>44367.0</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0.25</v>
+      </c>
       <c r="H9" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="13"/>
+      <c r="I9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -953,22 +1000,38 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
     </row>
-    <row r="10" ht="12.0" customHeight="1">
-      <c r="A10" s="6">
+    <row r="10" ht="41.25" customHeight="1">
+      <c r="A10" s="11">
         <v>8.0</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="8"/>
+      <c r="B10" s="13">
+        <v>44367.0</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.1</v>
+      </c>
       <c r="H10" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="6"/>
+      <c r="I10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
@@ -1001,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="13"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -1034,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="13"/>
+      <c r="J12" s="16"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -1056,18 +1119,18 @@
       <c r="A13" s="6">
         <v>11.0</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
@@ -1100,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="9"/>
-      <c r="J14" s="13"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -1133,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="13"/>
+      <c r="J15" s="16"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -1166,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="9"/>
-      <c r="J16" s="13"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>

</xml_diff>